<commit_message>
the last Update for R0
</commit_message>
<xml_diff>
--- a/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V1.xlsx
+++ b/R2/02_SignalMatrix/HkmcVehicleInpAdap/HkmcVehicleInputAdap_SignalMatrix_V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R2\02_SignalMatrix\HkmcVehicleInpAdap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E71FE0B-9B22-4924-A795-CCDF1F67AE96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4620F0D2-3B37-4EFD-9769-64440CC5ED6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="290">
   <si>
     <t>Change Log</t>
   </si>
@@ -141,16 +141,6 @@
     <t>Output</t>
   </si>
   <si>
-    <t>Cx0_AdasFCASR_Default
-Cx1_AdasFCASR_Off
-Cx2_AdasFCASR_Warning
-Cx3_AdasFCASR_Assist
-Cx4_AdasFCASR_Reserved
-Cx5_AdasFCASR_Reserved
-Cx6_AdasFCASR_Reserved
-Cx7_AdasFCASR_Invalid</t>
-  </si>
-  <si>
     <t>HVIA_MDPS</t>
   </si>
   <si>
@@ -193,228 +183,18 @@
     <t>HSYS_CLU_05_00ms</t>
   </si>
   <si>
-    <t>Cx0_AAsstSR_Default
-Cx1_AAsstSR_OFF
-Cx2_AAsstSR_Late
-Cx3_AAsstSR_Normal
-Cx4_AAsstSR_Early
-Cx5_AAsstSR_Reserved
-Cx6_AAsstSR_Reserved
-Cx7_AAsstSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_Fca1stWSR_Default
-Cx1_Fca1stWSR_On_Late
-Cx2_Fca1stWSR_ON_Normal
-Cx3_Fca1stWSR_ON_Early
-Cx4_Fca1stWSR_Reserved
-Cx5_Fca1stWSR_Reserved
-Cx6_Fca1stWSR_Reserved
-Cx7_Fca1stWSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_HADSR_Default
-Cx1_HADSR_Function_On
-Cx2_HADSR_Function_Off
-Cx3_HADSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_IslwSR_Default
-Cx1_IslwSR_Disable
-Cx2_IslwSR_Enable
-Cx3_IslwSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_StaR1R_Default
-Cx1_StaR1R_Reset
-Cx2_StaR1R_Not_Used
-Cx3_StaR1R_Error_Indicator</t>
-  </si>
-  <si>
     <t>HSYS_CLU_12_00ms</t>
   </si>
   <si>
-    <t>Cx0_AdasUSMRR_Default
-Cx1_AdasUSMRR_Reset
-Cx2_AdasUSMRR_Reserved
-Cx3_AdasUSMRR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasSCCDMSR_Default
-Cx1_AdasSCCDMSR_Comfort
-Cx2_AdasSCCDMSR_Normal
-Cx3_AdasSCCDMSR_Dynamic
-Cx4_AdasSCCDMSR_Reserved
-Cx5_AdasSCCDMSR_Reserved
-Cx6_AdasSCCDMSR_Reserved
-Cx7_AdasSCCDMSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasDAWMSR_Default
-Cx1_AdasDAWMSR_Off
-Cx2_AdasDAWMSR_Reserved
-Cx3_AdasDAWMSR_Normal
-Cx4_AdasDAWMSR_Early
-Cx5_AdasDAWMSR_Reserved
-Cx6_AdasDAWMSR_Reserved
-Cx7_AdasDAWMSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasHDASR_Default
-Cx1_AdasHDASR_Function_Off
-Cx2_AdasHDASR_Function_On
-Cx3_AdasHDASR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasNSCCCSR_Default
-Cx1_AdasNSCCCSR_Disable
-Cx2_AdasNSCCCSR_Enable
-Cx3_AdasNSCCCSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasLFASR_Default
-Cx1_AdasLFASR_Function_Off
-Cx2_AdasLFASR_Function_On
-Cx3_AdasLFASR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasBCASR_Default
-Cx1_AdasBCASR_Off
-Cx2_AdasBCASR_Warning
-Cx3_AdasBCASR_Assist
-Cx4_AdasBCASR_Reserved
-Cx5_AdasBCASR_Reserved
-Cx6_AdasBCASR_Reserved
-Cx7_AdasBCASR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasISLWSR_Default_x000D_
-Cx1_AdasISLWSR_Disable_x000D_
-Cx2_AdasISLWSR_Enable_x000D_
-Cx3_AdasISLWSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasWrngTSR_Default
-Cx1_AdasWrngTSR_Late
-Cx2_AdasWrngTSR_Normal
-Cx3_AdasWrngTSR_Reserved
-Cx4_AdasWrngTSR_Reserved
-Cx5_AdasWrngTSR_Reserved
-Cx6_AdasWrngTSR_Reserved
-Cx7_AdasWrngTSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasLVDASR_Default
-Cx1_AdasLVDASR_Off
-Cx2_AdasLVDASR_On
-Cx3_AdasLVDASR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasNSCCCSR_Default_x000D_
-Cx1_AdasNSCCCSR_Disable_x000D_
-Cx2_AdasNSCCCSR_Enable_x000D_
-Cx3_AdasNSCCCSR_Invalid</t>
-  </si>
-  <si>
     <t>HSYS_CLU_13_00ms</t>
   </si>
   <si>
-    <t>Cx0_AdasLkaMSR_Default
-Cx1_AdasLkaMSR_LDW_mode
-Cx2_AdasLkaMSR_LKA_mode
-Cx3_AdasLkaMSR_ACTIVE_LKA
-Cx4_AdasLkaMSR_LDW_ON
-Cx5_AdasLkaMSR_LDW_OFF
-Cx6_AdasLkaMSR_LDW/LKA_OFF
-Cx7_AdasLkaMSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasFCAJSR_Default
-Cx1_AdasFCAJSR_Off
-Cx2_AdasFCAJSR_On
-Cx3_AdasFCAJSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasHbaSR_Default
-Cx1_AdasHbaSR_Off
-Cx2_AdasHbaSR_On
-Cx3_AdasHbaSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasSCCMLSR_Default
-Cx1_AdasSCCMLSR_Off
-Cx2_AdasSCCMLSR_On
-Cx3_AdasSCCMLSR_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_AdasSCCMLRR_Default_x000D_
-Cx1_AdasSCCMLRR_Reset_x000D_
-Cx2_AdasSCCMLRR_Reserved_x000D_
-Cx3_AdasSCCMLRR_Invalid</t>
-  </si>
-  <si>
     <t>HSYS_MDPS_01_10ms</t>
   </si>
   <si>
-    <t>Cx0_LkaTAS_Deactivated
-Cx1_LkaTAS_Activated
-Cx2_LkaTAS_Not_Used
-Cx3_LkaTAS_Error_Indicator</t>
-  </si>
-  <si>
-    <t>Cx0_LkaTUS_Available
-Cx1_LkaTUS_Unavailable
-Cx2_LkaTUS_Not_used
-Cx3_LkaTUS_Error_Indicator</t>
-  </si>
-  <si>
-    <t>Cx0_LkaTFS_No_Fault
-Cx1_LkaTFS_Faulty
-Cx2_LkaTFS_Not_used
-Cx3_LkaTFS_Error_Indicator</t>
-  </si>
-  <si>
-    <t>Cx0_LkaFS_Not_Fail_State
-Cx1_LkaFS_Fail_State
-Cx2_LkaFS_Not_used
-Cx3_LkaFS_Error_Indicator</t>
-  </si>
-  <si>
-    <t>Cx0_FlxSS_Standard_Mode
-Cx1_FlxSS_Sport_Mode
-Cx2_FlxSS_Comfort_Mode
-Cx3_FlxSS_Reserved
-Cx4_FlxSS_Reserved
-Cx5_FlxSS_Reserved
-Cx6_FlxSS_Not_Used
-Cx7_FlxSS_Invalid</t>
-  </si>
-  <si>
-    <t>Cx0_CurrMV_Standard_Mode
-Cx1_CurrMV_Sport_Mode
-Cx2_CurrMV_Comfort_Mode
-Cx3_CurrMV_Reserved
-Cx4_CurrMV_Reserved
-Cx5_CurrMV_Reserved
-Cx6_CurrMV_Not_Used
-Cx7_CurrMV_Error_Indicator</t>
-  </si>
-  <si>
-    <t>Cx0_OutTV_Not_Used ; Cx1_OutTV_Error_Indicator</t>
-  </si>
-  <si>
-    <t>Cx0_StrTSV_Not_Used ; Cx1_StrTSV_Error_Indicator</t>
-  </si>
-  <si>
     <t>HSYS_BCM_08_200ms</t>
   </si>
   <si>
-    <t>Cx0_HbaCMT_HighControlMode_BCM
-Cx1_HbaCMT_HighControlMode_HBA
-Cx2_HbaCMT_Not_Used
-Cx3_HbaCMT_Error_Indicator</t>
-  </si>
-  <si>
     <t>HkmcVehicleInput SWC/VIPCDD SWC</t>
   </si>
   <si>
@@ -445,14 +225,6 @@
   </si>
   <si>
     <t>TopLevelCompostion</t>
-  </si>
-  <si>
-    <t>Cx0_Typ_C-MDPS
-Cx1_Typ_R-MDPS_Pinion
-Cx2_Typ_R-MDPS_Belt
-Cx6_Typ_Not_Used
-Cx7_Typ_Error_Indicator</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Cx0_SpdUT_kmperh
@@ -1491,6 +1263,268 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>BitLength:4, Factor : 1, BCM_AliveCounter8Value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>BitLength:8, Factor : 1, BCM_CyclicRedundancyCheck8Value</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AAsstSR_Default
+Cx1_AAsstSR_OFF
+Cx2_AAsstSR_Late
+Cx3_AAsstSR_Normal
+Cx4_AAsstSR_Early
+Cx5_AAsstSR_Reserved
+Cx6_AAsstSR_Reserved
+Cx7_AAsstSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_USMFca1stWSR_Default
+Cx1_USMFca1stWSR_On_Late
+Cx2_USMFca1stWSR_ON_Normal
+Cx3_USMFca1stWSR_ON_Early
+Cx4_USMFca1stWSR_Reserved
+Cx5_USMFca1stWSR_Reserved
+Cx6_USMFca1stWSR_Reserved
+Cx7_USMFca1stWSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_HADSR_Default
+Cx1_HADSR_Function_On
+Cx2_HADSR_Function_Off
+Cx3_HADSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_IslwSR_Default
+Cx1_IslwSR_Disable
+Cx2_IslwSR_Enable
+Cx3_IslwSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_StaR1R_Default
+Cx1_StaR1R_Reset
+Cx2_StaR1R_Not_Used
+Cx3_StaR1R_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasUSMRR_Default
+Cx1_AdasUSMRR_Reset
+Cx2_AdasUSMRR_Reserved
+Cx3_AdasUSMRR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasFCASR_Default
+Cx1_AdasFCASR_Off
+Cx2_AdasFCASR_Warning
+Cx3_AdasFCASR_Assist
+Cx4_AdasFCASR_Reserved
+Cx5_AdasFCASR_Reserved
+Cx6_AdasFCASR_Reserved
+Cx7_AdasFCASR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasSCCDMSR_Default
+Cx1_AdasSCCDMSR_Comfort
+Cx2_AdasSCCDMSR_Normal
+Cx3_AdasSCCDMSR_Dynamic
+Cx4_AdasSCCDMSR_Reserved
+Cx5_AdasSCCDMSR_Reserved
+Cx6_AdasSCCDMSR_Reserved
+Cx7_AdasSCCDMSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasDAWMSR_Default
+Cx1_AdasDAWMSR_Off
+Cx2_AdasDAWMSR_Reserved
+Cx3_AdasDAWMSR_Normal
+Cx4_AdasDAWMSR_Early
+Cx5_AdasDAWMSR_Reserved
+Cx6_AdasDAWMSR_Reserved
+Cx7_AdasDAWMSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasHDASR_Default
+Cx1_AdasHDASR_Function_Off
+Cx2_AdasHDASR_Function_On
+Cx3_AdasHDASR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasNSCCCSR_Default
+Cx1_AdasNSCCCSR_Disable
+Cx2_AdasNSCCCSR_Enable
+Cx3_AdasNSCCCSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasLFASR_Default
+Cx1_AdasLFASR_Function_Off
+Cx2_AdasLFASR_Function_On
+Cx3_AdasLFASR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasBCASR_Default
+Cx1_AdasBCASR_Off
+Cx2_AdasBCASR_Warning
+Cx3_AdasBCASR_Assist
+Cx4_AdasBCASR_Reserved
+Cx5_AdasBCASR_Reserved
+Cx6_AdasBCASR_Reserved
+Cx7_AdasBCASR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasISLWSR_Default
+Cx1_AdasISLWSR_Disable
+Cx2_AdasISLWSR_Enable
+Cx3_AdasISLWSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasWrngTSR_Default
+Cx1_AdasWrngTSR_Late
+Cx2_AdasWrngTSR_Normal
+Cx3_AdasWrngTSR_Reserved
+Cx4_AdasWrngTSR_Reserved
+Cx5_AdasWrngTSR_Reserved
+Cx6_AdasWrngTSR_Reserved
+Cx7_AdasWrngTSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasLVDASR_Default
+Cx1_AdasLVDASR_Off
+Cx2_AdasLVDASR_On
+Cx3_AdasLVDASR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasLkaMSR_Default
+Cx1_AdasLkaMSR_LDW_mode
+Cx2_AdasLkaMSR_LKA_mode
+Cx3_AdasLkaMSR_ACTIVE_LKA
+Cx4_AdasLkaMSR_LDW_ON
+Cx5_AdasLkaMSR_LDW_OFF
+Cx6_AdasLkaMSR_LDW_LKA_OFF
+Cx7_AdasLkaMSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasFCAJSR_Default
+Cx1_AdasFCAJSR_Off
+Cx2_AdasFCAJSR_On
+Cx3_AdasFCAJSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasHbaSR_Default
+Cx1_AdasHbaSR_Off
+Cx2_AdasHbaSR_On
+Cx3_AdasHbaSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasSCCMLSR_Default
+Cx1_AdasSCCMLSR_Off
+Cx2_AdasSCCMLSR_On
+Cx3_AdasSCCMLSR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_AdasSCCMLRR_Default
+Cx1_AdasSCCMLRR_Reset
+Cx2_AdasSCCMLRR_Reserved
+Cx3_AdasSCCMLRR_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_Typ_C_MDPS
+Cx1_Typ_R_MDPS_Pinion
+Cx2_Typ_R_MDPS_Belt
+Cx6_Typ_Not_Used
+Cx7_Typ_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LkaTAS_Deactivated
+Cx1_LkaTAS_Activated
+Cx2_LkaTAS_Not_Used
+Cx3_LkaTAS_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LkaTUS_Available
+Cx1_LkaTUS_Unavailable
+Cx2_LkaTUS_Not_used
+Cx3_LkaTUS_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LkaTFS_No_Fault
+Cx1_LkaTFS_Faulty
+Cx2_LkaTFS_Not_used
+Cx3_LkaTFS_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_FlxSS_Standard_Mode
+Cx1_FlxSS_Sport_Mode
+Cx2_FlxSS_Comfort_Mode
+Cx3_FlxSS_Reserved
+Cx4_FlxSS_Reserved
+Cx5_FlxSS_Reserved
+Cx6_FlxSS_Not_Used
+Cx7_FlxSS_Invalid</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_CurrMV_Standard_Mode
+Cx1_CurrMV_Sport_Mode
+Cx2_CurrMV_Comfort_Mode
+Cx3_CurrMV_Reserved
+Cx4_CurrMV_Reserved
+Cx5_CurrMV_Reserved
+Cx6_CurrMV_Not_Used
+Cx7_CurrMV_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_OutTV_Not_Used
+Cx1_OutTV_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_StrTSV_Not_Used
+Cx1_StrTSV_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_HbaCMT_HighControlMode_BCM
+Cx1_HbaCMT_HighControlMode_HBA
+Cx2_HbaCMT_Not_Used
+Cx3_HbaCMT_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cx0_LkaFS_Not_Fail_State
+Cx1_LkaFS_Fail_State
+Cx2_LkaFS_Not_used
+Cx3_LkaFS_Error_Indicator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Cx0_PMS_Reserved
 Cx1_PMS_Steering_still_in_initialization_phase
 Cx2_PMS_Steering_ready_waits_for_PA_command
@@ -1499,16 +1533,8 @@
 Cx5_PMS_Steering_requested_to_go_to_final_activation_step
 Cx6_PMS_Steering_went_to_error_internally
 Cx7_PMS_Steering_aborted_the_automatic_function
-0xE_PMS_Not_Used
-0xF_PMS_Error_Indicator</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BitLength:4, Factor : 1, BCM_AliveCounter8Value</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>BitLength:8, Factor : 1, BCM_CyclicRedundancyCheck8Value</t>
+CxE_PMS_Not_Used
+CxF_PMS_Error_Indicator</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4327,10 +4353,10 @@
   <dimension ref="A1:Y120"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S116" sqref="S116"/>
+      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -4429,10 +4455,10 @@
         <v>1</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="P2" s="40" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="Q2" s="40" t="s">
         <v>18</v>
@@ -4441,7 +4467,7 @@
         <v>19</v>
       </c>
       <c r="S2" s="53" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="T2" s="41"/>
       <c r="U2" s="41"/>
@@ -4471,7 +4497,7 @@
         <v>17</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="Q3" s="40" t="s">
         <v>18</v>
@@ -4480,7 +4506,7 @@
         <v>19</v>
       </c>
       <c r="S3" s="53" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="T3" s="41"/>
       <c r="U3" s="41"/>
@@ -4510,7 +4536,7 @@
         <v>17</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="Q4" s="40" t="s">
         <v>18</v>
@@ -4519,7 +4545,7 @@
         <v>19</v>
       </c>
       <c r="S4" s="53" t="s">
-        <v>249</v>
+        <v>217</v>
       </c>
       <c r="T4" s="41"/>
       <c r="U4" s="41"/>
@@ -4546,10 +4572,10 @@
         <v>4</v>
       </c>
       <c r="O5" s="39" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="P5" s="40" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
       <c r="Q5" s="40" t="s">
         <v>18</v>
@@ -4558,7 +4584,7 @@
         <v>19</v>
       </c>
       <c r="S5" s="53" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
       <c r="T5" s="41"/>
       <c r="U5" s="41"/>
@@ -4588,7 +4614,7 @@
         <v>17</v>
       </c>
       <c r="P6" s="40" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="Q6" s="40" t="s">
         <v>18</v>
@@ -4597,7 +4623,7 @@
         <v>19</v>
       </c>
       <c r="S6" s="53" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
       <c r="T6" s="41"/>
       <c r="U6" s="41"/>
@@ -4624,10 +4650,10 @@
         <v>6</v>
       </c>
       <c r="O7" s="39" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="P7" s="40" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="Q7" s="40" t="s">
         <v>18</v>
@@ -4636,7 +4662,7 @@
         <v>19</v>
       </c>
       <c r="S7" s="53" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="T7" s="41"/>
       <c r="U7" s="41"/>
@@ -4663,10 +4689,10 @@
         <v>7</v>
       </c>
       <c r="O8" s="39" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="Q8" s="40" t="s">
         <v>18</v>
@@ -4675,7 +4701,7 @@
         <v>19</v>
       </c>
       <c r="S8" s="53" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="T8" s="41"/>
       <c r="U8" s="41"/>
@@ -4700,7 +4726,7 @@
       <c r="M9" s="49"/>
       <c r="N9" s="52"/>
       <c r="O9" s="28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
@@ -4729,19 +4755,19 @@
       <c r="M10" s="49"/>
       <c r="N10" s="52"/>
       <c r="O10" s="64" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="P10" s="54" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
       <c r="Q10" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R10" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S10" s="55" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="T10" s="41"/>
       <c r="U10" s="41"/>
@@ -4760,16 +4786,16 @@
       <c r="N11" s="52"/>
       <c r="O11" s="65"/>
       <c r="P11" s="54" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R11" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S11" s="55" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:25" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4779,16 +4805,16 @@
       <c r="N12" s="52"/>
       <c r="O12" s="65"/>
       <c r="P12" s="54" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R12" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S12" s="55" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4798,13 +4824,13 @@
       <c r="N13" s="52"/>
       <c r="O13" s="65"/>
       <c r="P13" s="54" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="Q13" s="54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R13" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S13" s="55"/>
     </row>
@@ -4815,16 +4841,16 @@
       <c r="N14" s="52"/>
       <c r="O14" s="65"/>
       <c r="P14" s="73" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
       <c r="Q14" s="73" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="R14" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S14" s="75" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4834,13 +4860,13 @@
       <c r="N15" s="52"/>
       <c r="O15" s="65"/>
       <c r="P15" s="54" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="Q15" s="54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R15" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S15" s="55"/>
     </row>
@@ -4851,16 +4877,16 @@
       <c r="N16" s="52"/>
       <c r="O16" s="65"/>
       <c r="P16" s="54" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="Q16" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R16" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S16" s="55" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="6:19" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4870,16 +4896,16 @@
       <c r="N17" s="52"/>
       <c r="O17" s="65"/>
       <c r="P17" s="54" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="Q17" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R17" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S17" s="55" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="6:19" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4889,16 +4915,16 @@
       <c r="N18" s="52"/>
       <c r="O18" s="65"/>
       <c r="P18" s="54" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="Q18" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R18" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S18" s="55" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="6:19" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4908,13 +4934,13 @@
       <c r="N19" s="52"/>
       <c r="O19" s="66"/>
       <c r="P19" s="54" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="Q19" s="54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R19" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S19" s="55"/>
     </row>
@@ -4929,19 +4955,19 @@
       <c r="M20" s="49"/>
       <c r="N20" s="52"/>
       <c r="O20" s="64" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="P20" s="54" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="Q20" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R20" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S20" s="55" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4950,16 +4976,16 @@
       <c r="N21" s="52"/>
       <c r="O21" s="65"/>
       <c r="P21" s="54" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="Q21" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R21" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S21" s="55" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4968,16 +4994,16 @@
       <c r="N22" s="52"/>
       <c r="O22" s="65"/>
       <c r="P22" s="54" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="Q22" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R22" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S22" s="55" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -4992,16 +5018,16 @@
       <c r="N23" s="52"/>
       <c r="O23" s="65"/>
       <c r="P23" s="54" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="Q23" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R23" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S23" s="55" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5010,16 +5036,16 @@
       <c r="N24" s="52"/>
       <c r="O24" s="65"/>
       <c r="P24" s="54" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="Q24" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R24" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S24" s="55" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5028,16 +5054,16 @@
       <c r="N25" s="52"/>
       <c r="O25" s="65"/>
       <c r="P25" s="54" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="Q25" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R25" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S25" s="55" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5052,16 +5078,16 @@
       <c r="N26" s="52"/>
       <c r="O26" s="65"/>
       <c r="P26" s="54" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="Q26" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R26" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S26" s="55" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5070,16 +5096,16 @@
       <c r="N27" s="52"/>
       <c r="O27" s="65"/>
       <c r="P27" s="54" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="Q27" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R27" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S27" s="55" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5088,16 +5114,16 @@
       <c r="N28" s="52"/>
       <c r="O28" s="65"/>
       <c r="P28" s="54" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="Q28" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R28" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S28" s="55" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5106,16 +5132,16 @@
       <c r="N29" s="52"/>
       <c r="O29" s="66"/>
       <c r="P29" s="54" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="Q29" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R29" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S29" s="55" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5129,19 +5155,19 @@
       <c r="M30" s="49"/>
       <c r="N30" s="52"/>
       <c r="O30" s="64" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="P30" s="54" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="Q30" s="54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R30" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S30" s="55" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5150,16 +5176,16 @@
       <c r="N31" s="52"/>
       <c r="O31" s="65"/>
       <c r="P31" s="54" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="Q31" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R31" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S31" s="55" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5168,16 +5194,16 @@
       <c r="N32" s="52"/>
       <c r="O32" s="65"/>
       <c r="P32" s="54" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="Q32" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R32" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S32" s="55" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5186,16 +5212,16 @@
       <c r="N33" s="52"/>
       <c r="O33" s="65"/>
       <c r="P33" s="54" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="Q33" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R33" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S33" s="55" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5204,16 +5230,16 @@
       <c r="N34" s="52"/>
       <c r="O34" s="65"/>
       <c r="P34" s="54" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="Q34" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R34" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S34" s="55" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5222,16 +5248,16 @@
       <c r="N35" s="52"/>
       <c r="O35" s="65"/>
       <c r="P35" s="54" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="Q35" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R35" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S35" s="55" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5240,16 +5266,16 @@
       <c r="N36" s="52"/>
       <c r="O36" s="65"/>
       <c r="P36" s="54" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="Q36" s="54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R36" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S36" s="55" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5258,13 +5284,13 @@
       <c r="N37" s="52"/>
       <c r="O37" s="65"/>
       <c r="P37" s="54" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="Q37" s="54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R37" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S37" s="55"/>
     </row>
@@ -5274,16 +5300,16 @@
       <c r="N38" s="52"/>
       <c r="O38" s="65"/>
       <c r="P38" s="54" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="Q38" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R38" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S38" s="55" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5292,13 +5318,13 @@
       <c r="N39" s="52"/>
       <c r="O39" s="65"/>
       <c r="P39" s="54" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="Q39" s="54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R39" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S39" s="56"/>
     </row>
@@ -5308,13 +5334,13 @@
       <c r="N40" s="52"/>
       <c r="O40" s="66"/>
       <c r="P40" s="54" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="Q40" s="54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R40" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S40" s="56"/>
     </row>
@@ -5323,19 +5349,19 @@
       <c r="H41" s="51"/>
       <c r="N41" s="52"/>
       <c r="O41" s="64" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
       <c r="P41" s="32" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="Q41" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R41" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S41" s="55" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5344,16 +5370,16 @@
       <c r="N42" s="52"/>
       <c r="O42" s="65"/>
       <c r="P42" s="32" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="Q42" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R42" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S42" s="55" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5362,16 +5388,16 @@
       <c r="N43" s="52"/>
       <c r="O43" s="65"/>
       <c r="P43" s="32" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="Q43" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R43" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S43" s="55" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5380,16 +5406,16 @@
       <c r="N44" s="52"/>
       <c r="O44" s="65"/>
       <c r="P44" s="32" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="Q44" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R44" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S44" s="55" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5398,16 +5424,16 @@
       <c r="N45" s="52"/>
       <c r="O45" s="65"/>
       <c r="P45" s="32" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="Q45" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R45" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S45" s="55" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5416,16 +5442,16 @@
       <c r="N46" s="52"/>
       <c r="O46" s="65"/>
       <c r="P46" s="32" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="Q46" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R46" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S46" s="55" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
     </row>
     <row r="47" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5434,16 +5460,16 @@
       <c r="N47" s="52"/>
       <c r="O47" s="65"/>
       <c r="P47" s="32" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="Q47" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R47" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S47" s="55" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5452,16 +5478,16 @@
       <c r="N48" s="52"/>
       <c r="O48" s="65"/>
       <c r="P48" s="32" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="Q48" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R48" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S48" s="55" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5470,16 +5496,16 @@
       <c r="N49" s="52"/>
       <c r="O49" s="65"/>
       <c r="P49" s="32" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="Q49" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R49" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S49" s="55" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5488,16 +5514,16 @@
       <c r="N50" s="52"/>
       <c r="O50" s="65"/>
       <c r="P50" s="32" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="Q50" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R50" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S50" s="55" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5506,16 +5532,16 @@
       <c r="N51" s="52"/>
       <c r="O51" s="65"/>
       <c r="P51" s="54" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
       <c r="Q51" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R51" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S51" s="55" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5524,16 +5550,16 @@
       <c r="N52" s="52"/>
       <c r="O52" s="65"/>
       <c r="P52" s="32" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="Q52" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R52" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S52" s="55" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5542,16 +5568,16 @@
       <c r="N53" s="52"/>
       <c r="O53" s="65"/>
       <c r="P53" s="58" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="Q53" s="59" t="s">
         <v>18</v>
       </c>
       <c r="R53" s="59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S53" s="60" t="s">
-        <v>253</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5560,16 +5586,16 @@
       <c r="N54" s="52"/>
       <c r="O54" s="65"/>
       <c r="P54" s="32" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="Q54" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R54" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S54" s="55" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5578,16 +5604,16 @@
       <c r="N55" s="52"/>
       <c r="O55" s="65"/>
       <c r="P55" s="32" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
       <c r="Q55" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R55" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S55" s="55" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5596,16 +5622,16 @@
       <c r="N56" s="52"/>
       <c r="O56" s="65"/>
       <c r="P56" s="32" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
       <c r="Q56" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R56" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S56" s="55" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5614,16 +5640,16 @@
       <c r="N57" s="52"/>
       <c r="O57" s="65"/>
       <c r="P57" s="32" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="Q57" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R57" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S57" s="55" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5632,16 +5658,16 @@
       <c r="N58" s="52"/>
       <c r="O58" s="65"/>
       <c r="P58" s="32" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="Q58" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R58" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S58" s="55" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5650,16 +5676,16 @@
       <c r="N59" s="52"/>
       <c r="O59" s="65"/>
       <c r="P59" s="32" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
       <c r="Q59" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R59" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S59" s="55" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5668,16 +5694,16 @@
       <c r="N60" s="52"/>
       <c r="O60" s="65"/>
       <c r="P60" s="32" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="Q60" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R60" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S60" s="55" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5686,16 +5712,16 @@
       <c r="N61" s="52"/>
       <c r="O61" s="65"/>
       <c r="P61" s="32" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
       <c r="Q61" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R61" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S61" s="55" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5704,16 +5730,16 @@
       <c r="N62" s="52"/>
       <c r="O62" s="65"/>
       <c r="P62" s="32" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="Q62" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R62" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S62" s="55" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5722,16 +5748,16 @@
       <c r="N63" s="52"/>
       <c r="O63" s="65"/>
       <c r="P63" s="32" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="Q63" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R63" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S63" s="55" t="s">
-        <v>263</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5740,16 +5766,16 @@
       <c r="N64" s="52"/>
       <c r="O64" s="65"/>
       <c r="P64" s="32" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="Q64" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R64" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S64" s="55" t="s">
-        <v>264</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5758,16 +5784,16 @@
       <c r="N65" s="52"/>
       <c r="O65" s="65"/>
       <c r="P65" s="32" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="Q65" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R65" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S65" s="55" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
     </row>
     <row r="66" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5776,16 +5802,16 @@
       <c r="N66" s="52"/>
       <c r="O66" s="65"/>
       <c r="P66" s="54" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="Q66" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R66" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S66" s="55" t="s">
-        <v>266</v>
+        <v>234</v>
       </c>
     </row>
     <row r="67" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5794,16 +5820,16 @@
       <c r="N67" s="52"/>
       <c r="O67" s="65"/>
       <c r="P67" s="32" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="Q67" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R67" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S67" s="55" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5812,16 +5838,16 @@
       <c r="N68" s="52"/>
       <c r="O68" s="65"/>
       <c r="P68" s="32" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="Q68" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R68" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S68" s="55" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
     </row>
     <row r="69" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5830,16 +5856,16 @@
       <c r="N69" s="52"/>
       <c r="O69" s="65"/>
       <c r="P69" s="32" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="Q69" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R69" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S69" s="55" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
     </row>
     <row r="70" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5854,16 +5880,16 @@
       <c r="N70" s="52"/>
       <c r="O70" s="66"/>
       <c r="P70" s="58" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="Q70" s="59" t="s">
         <v>18</v>
       </c>
       <c r="R70" s="59" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S70" s="60" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5877,7 +5903,7 @@
       <c r="M71" s="49"/>
       <c r="N71" s="52"/>
       <c r="O71" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P71" s="33"/>
       <c r="Q71" s="29"/>
@@ -5895,19 +5921,19 @@
       <c r="M72" s="49"/>
       <c r="N72" s="52"/>
       <c r="O72" s="64" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="P72" s="73" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
       <c r="Q72" s="73" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="R72" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S72" s="74" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
     </row>
     <row r="73" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5916,16 +5942,16 @@
       <c r="N73" s="52"/>
       <c r="O73" s="65"/>
       <c r="P73" s="73" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="Q73" s="73" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="R73" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S73" s="74" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
     </row>
     <row r="74" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5934,16 +5960,16 @@
       <c r="N74" s="52"/>
       <c r="O74" s="65"/>
       <c r="P74" s="54" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
       <c r="Q74" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R74" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S74" s="55" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5952,16 +5978,16 @@
       <c r="N75" s="52"/>
       <c r="O75" s="65"/>
       <c r="P75" s="54" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
       <c r="Q75" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R75" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S75" s="55" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
     </row>
     <row r="76" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5970,16 +5996,16 @@
       <c r="N76" s="52"/>
       <c r="O76" s="65"/>
       <c r="P76" s="54" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="Q76" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R76" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S76" s="55" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -5988,16 +6014,16 @@
       <c r="N77" s="52"/>
       <c r="O77" s="65"/>
       <c r="P77" s="54" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="Q77" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R77" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S77" s="55" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6006,16 +6032,16 @@
       <c r="N78" s="52"/>
       <c r="O78" s="66"/>
       <c r="P78" s="73" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="Q78" s="73" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="R78" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S78" s="76" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
     </row>
     <row r="79" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6029,19 +6055,19 @@
       <c r="M79" s="49"/>
       <c r="N79" s="52"/>
       <c r="O79" s="64" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="P79" s="54" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="Q79" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R79" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S79" s="55" t="s">
-        <v>35</v>
+        <v>258</v>
       </c>
     </row>
     <row r="80" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6050,16 +6076,16 @@
       <c r="N80" s="52"/>
       <c r="O80" s="65"/>
       <c r="P80" s="54" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="Q80" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R80" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="S80" s="55" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="S80" s="75" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="81" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6068,16 +6094,16 @@
       <c r="N81" s="52"/>
       <c r="O81" s="65"/>
       <c r="P81" s="54" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="Q81" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R81" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S81" s="55" t="s">
-        <v>37</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6086,16 +6112,16 @@
       <c r="N82" s="52"/>
       <c r="O82" s="65"/>
       <c r="P82" s="54" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="Q82" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R82" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S82" s="55" t="s">
-        <v>38</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6104,16 +6130,16 @@
       <c r="N83" s="52"/>
       <c r="O83" s="66"/>
       <c r="P83" s="54" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="Q83" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R83" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S83" s="55" t="s">
-        <v>39</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6127,19 +6153,19 @@
       <c r="M84" s="49"/>
       <c r="N84" s="52"/>
       <c r="O84" s="64" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="P84" s="73" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="Q84" s="73" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="R84" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S84" s="76" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
     </row>
     <row r="85" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6148,16 +6174,16 @@
       <c r="N85" s="52"/>
       <c r="O85" s="65"/>
       <c r="P85" s="73" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
       <c r="Q85" s="73" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="R85" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S85" s="75" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
     </row>
     <row r="86" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6166,16 +6192,16 @@
       <c r="N86" s="52"/>
       <c r="O86" s="65"/>
       <c r="P86" s="54" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
       <c r="Q86" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R86" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S86" s="55" t="s">
-        <v>41</v>
+        <v>263</v>
       </c>
     </row>
     <row r="87" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6184,16 +6210,16 @@
       <c r="N87" s="52"/>
       <c r="O87" s="65"/>
       <c r="P87" s="54" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="Q87" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R87" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S87" s="55" t="s">
-        <v>20</v>
+        <v>264</v>
       </c>
     </row>
     <row r="88" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6202,16 +6228,16 @@
       <c r="N88" s="52"/>
       <c r="O88" s="65"/>
       <c r="P88" s="54" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="Q88" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R88" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S88" s="55" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6220,16 +6246,16 @@
       <c r="N89" s="52"/>
       <c r="O89" s="65"/>
       <c r="P89" s="54" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
       <c r="Q89" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R89" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S89" s="55" t="s">
-        <v>43</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6238,16 +6264,16 @@
       <c r="N90" s="52"/>
       <c r="O90" s="65"/>
       <c r="P90" s="54" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="Q90" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R90" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S90" s="55" t="s">
-        <v>44</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6256,16 +6282,16 @@
       <c r="N91" s="52"/>
       <c r="O91" s="65"/>
       <c r="P91" s="54" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="Q91" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R91" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S91" s="55" t="s">
-        <v>45</v>
+        <v>268</v>
       </c>
     </row>
     <row r="92" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6274,16 +6300,16 @@
       <c r="N92" s="52"/>
       <c r="O92" s="65"/>
       <c r="P92" s="54" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="Q92" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R92" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S92" s="55" t="s">
-        <v>46</v>
+        <v>269</v>
       </c>
     </row>
     <row r="93" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6292,16 +6318,16 @@
       <c r="N93" s="52"/>
       <c r="O93" s="65"/>
       <c r="P93" s="54" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
       <c r="Q93" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R93" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S93" s="55" t="s">
-        <v>47</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6310,16 +6336,16 @@
       <c r="N94" s="52"/>
       <c r="O94" s="65"/>
       <c r="P94" s="54" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="Q94" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R94" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S94" s="55" t="s">
-        <v>48</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6328,16 +6354,16 @@
       <c r="N95" s="52"/>
       <c r="O95" s="65"/>
       <c r="P95" s="54" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="Q95" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R95" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S95" s="55" t="s">
-        <v>49</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6346,16 +6372,16 @@
       <c r="N96" s="52"/>
       <c r="O96" s="65"/>
       <c r="P96" s="54" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="Q96" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R96" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S96" s="55" t="s">
-        <v>50</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6364,16 +6390,16 @@
       <c r="N97" s="52"/>
       <c r="O97" s="66"/>
       <c r="P97" s="54" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="Q97" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R97" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S97" s="55" t="s">
-        <v>51</v>
+        <v>268</v>
       </c>
     </row>
     <row r="98" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6387,19 +6413,19 @@
       <c r="M98" s="49"/>
       <c r="N98" s="52"/>
       <c r="O98" s="64" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="P98" s="73" t="s">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="Q98" s="73" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="R98" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S98" s="76" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
     </row>
     <row r="99" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6408,16 +6434,16 @@
       <c r="N99" s="52"/>
       <c r="O99" s="65"/>
       <c r="P99" s="73" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
       <c r="Q99" s="73" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="R99" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S99" s="76" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
     </row>
     <row r="100" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6426,16 +6452,16 @@
       <c r="N100" s="52"/>
       <c r="O100" s="65"/>
       <c r="P100" s="54" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="Q100" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R100" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="S100" s="55" t="s">
-        <v>53</v>
+        <v>23</v>
+      </c>
+      <c r="S100" s="75" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6444,16 +6470,16 @@
       <c r="N101" s="52"/>
       <c r="O101" s="65"/>
       <c r="P101" s="54" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="Q101" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R101" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S101" s="55" t="s">
-        <v>54</v>
+        <v>275</v>
       </c>
     </row>
     <row r="102" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6462,16 +6488,16 @@
       <c r="N102" s="52"/>
       <c r="O102" s="65"/>
       <c r="P102" s="54" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
       <c r="Q102" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R102" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S102" s="55" t="s">
-        <v>55</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6480,16 +6506,16 @@
       <c r="N103" s="52"/>
       <c r="O103" s="65"/>
       <c r="P103" s="54" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="Q103" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R103" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S103" s="55" t="s">
-        <v>56</v>
+        <v>277</v>
       </c>
     </row>
     <row r="104" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6498,16 +6524,16 @@
       <c r="N104" s="52"/>
       <c r="O104" s="66"/>
       <c r="P104" s="54" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="Q104" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R104" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S104" s="55" t="s">
-        <v>57</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6521,19 +6547,19 @@
       <c r="M105" s="49"/>
       <c r="N105" s="52"/>
       <c r="O105" s="64" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
       <c r="P105" s="73" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="Q105" s="73" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="R105" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S105" s="76" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
     </row>
     <row r="106" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6542,16 +6568,16 @@
       <c r="N106" s="52"/>
       <c r="O106" s="65"/>
       <c r="P106" s="73" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="Q106" s="73" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="R106" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S106" s="76" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
     </row>
     <row r="107" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6560,16 +6586,16 @@
       <c r="N107" s="52"/>
       <c r="O107" s="65"/>
       <c r="P107" s="54" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
       <c r="Q107" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R107" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S107" s="55" t="s">
-        <v>79</v>
+        <v>279</v>
       </c>
     </row>
     <row r="108" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6578,16 +6604,16 @@
       <c r="N108" s="52"/>
       <c r="O108" s="65"/>
       <c r="P108" s="73" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="Q108" s="73" t="s">
         <v>18</v>
       </c>
       <c r="R108" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S108" s="75" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="109" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6596,16 +6622,16 @@
       <c r="N109" s="52"/>
       <c r="O109" s="65"/>
       <c r="P109" s="54" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
       <c r="Q109" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R109" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S109" s="55" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
     </row>
     <row r="110" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6614,16 +6640,16 @@
       <c r="N110" s="52"/>
       <c r="O110" s="65"/>
       <c r="P110" s="54" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="Q110" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R110" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S110" s="55" t="s">
-        <v>59</v>
+        <v>280</v>
       </c>
     </row>
     <row r="111" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6632,16 +6658,16 @@
       <c r="N111" s="52"/>
       <c r="O111" s="65"/>
       <c r="P111" s="54" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="Q111" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R111" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S111" s="55" t="s">
-        <v>60</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6650,16 +6676,16 @@
       <c r="N112" s="52"/>
       <c r="O112" s="65"/>
       <c r="P112" s="54" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="Q112" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R112" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S112" s="55" t="s">
-        <v>61</v>
+        <v>282</v>
       </c>
     </row>
     <row r="113" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6668,16 +6694,16 @@
       <c r="N113" s="52"/>
       <c r="O113" s="65"/>
       <c r="P113" s="54" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="Q113" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R113" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S113" s="55" t="s">
-        <v>62</v>
+        <v>288</v>
       </c>
     </row>
     <row r="114" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6686,16 +6712,16 @@
       <c r="N114" s="52"/>
       <c r="O114" s="65"/>
       <c r="P114" s="54" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="Q114" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R114" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S114" s="55" t="s">
-        <v>63</v>
+        <v>283</v>
       </c>
     </row>
     <row r="115" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6704,16 +6730,16 @@
       <c r="N115" s="52"/>
       <c r="O115" s="65"/>
       <c r="P115" s="54" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="Q115" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R115" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S115" s="55" t="s">
-        <v>64</v>
+        <v>284</v>
       </c>
     </row>
     <row r="116" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6722,16 +6748,16 @@
       <c r="N116" s="52"/>
       <c r="O116" s="65"/>
       <c r="P116" s="54" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="Q116" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R116" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S116" s="55" t="s">
-        <v>65</v>
+        <v>285</v>
       </c>
     </row>
     <row r="117" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6740,16 +6766,16 @@
       <c r="N117" s="52"/>
       <c r="O117" s="66"/>
       <c r="P117" s="54" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="Q117" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R117" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S117" s="55" t="s">
-        <v>66</v>
+        <v>286</v>
       </c>
     </row>
     <row r="118" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6763,19 +6789,19 @@
       <c r="M118" s="49"/>
       <c r="N118" s="52"/>
       <c r="O118" s="64" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="P118" s="73" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="Q118" s="73" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="R118" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S118" s="74" t="s">
-        <v>290</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="6:19" s="49" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6784,16 +6810,16 @@
       <c r="N119" s="52"/>
       <c r="O119" s="65"/>
       <c r="P119" s="73" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="Q119" s="73" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="R119" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S119" s="74" t="s">
-        <v>289</v>
+        <v>256</v>
       </c>
     </row>
     <row r="120" spans="6:19" s="27" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -6808,16 +6834,16 @@
       <c r="N120" s="52"/>
       <c r="O120" s="66"/>
       <c r="P120" s="54" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="Q120" s="54" t="s">
         <v>18</v>
       </c>
       <c r="R120" s="54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S120" s="55" t="s">
-        <v>68</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -6873,11 +6899,11 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="68" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
@@ -6887,21 +6913,21 @@
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="44" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="41" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>17</v>
@@ -6910,33 +6936,33 @@
         <v>19</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" s="41" customFormat="1" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="F4" s="43"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>19</v>
@@ -6944,7 +6970,7 @@
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -6995,11 +7021,11 @@
   <sheetData>
     <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="68" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="D1" s="69"/>
       <c r="E1" s="69"/>
@@ -7016,51 +7042,51 @@
       <c r="A2" s="67"/>
       <c r="B2" s="67"/>
       <c r="C2" s="44" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="44" t="s">
-        <v>28</v>
-      </c>
       <c r="G2" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="44" t="s">
+      <c r="J2" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="44" t="s">
-        <v>40</v>
-      </c>
       <c r="K2" s="44" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="L2" s="44" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="M2" s="44" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="70" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
@@ -7075,14 +7101,14 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="71"/>
       <c r="B4" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="43"/>
       <c r="E4" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="F4" s="43"/>
       <c r="G4" s="43"/>
@@ -7096,15 +7122,15 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="71"/>
       <c r="B5" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
@@ -7117,16 +7143,16 @@
     <row r="6" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="71"/>
       <c r="B6" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
@@ -7138,17 +7164,17 @@
     <row r="7" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="71"/>
       <c r="B7" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
       <c r="H7" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -7159,10 +7185,10 @@
     <row r="8" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="71"/>
       <c r="B8" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -7170,7 +7196,7 @@
       <c r="G8" s="43"/>
       <c r="H8" s="43"/>
       <c r="I8" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="J8" s="43"/>
       <c r="K8" s="43"/>
@@ -7180,10 +7206,10 @@
     <row r="9" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="71"/>
       <c r="B9" s="46" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="43"/>
       <c r="E9" s="43"/>
@@ -7192,7 +7218,7 @@
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="K9" s="43"/>
       <c r="L9" s="43"/>
@@ -7201,10 +7227,10 @@
     <row r="10" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="71"/>
       <c r="B10" s="46" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
@@ -7214,7 +7240,7 @@
       <c r="I10" s="43"/>
       <c r="J10" s="43"/>
       <c r="K10" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="L10" s="43"/>
       <c r="M10" s="43"/>
@@ -7222,10 +7248,10 @@
     <row r="11" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="71"/>
       <c r="B11" s="46" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
@@ -7236,17 +7262,17 @@
       <c r="J11" s="43"/>
       <c r="K11" s="43"/>
       <c r="L11" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="72"/>
       <c r="B12" s="46" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
@@ -7258,7 +7284,7 @@
       <c r="K12" s="43"/>
       <c r="L12" s="43"/>
       <c r="M12" s="43" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -7517,16 +7543,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a0b74ea9-89d9-43cb-a163-e9320d483776"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="800f79bc-e7dd-46fb-9ad5-c233bb1abdf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>